<commit_message>
Update the annotation status
</commit_message>
<xml_diff>
--- a/annotation_status.xlsx
+++ b/annotation_status.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="47">
   <si>
     <t xml:space="preserve">FileName</t>
   </si>
@@ -101,6 +101,66 @@
   </si>
   <si>
     <t xml:space="preserve">plate7rep1_20200426_103425_693_WellD09_PointD09_0007_ChannelDAPI,WF_GFP,TRITC,WF_Cy5,DIA_Seq0349.h5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plateK10rep1_20200429_122048_065_WellA06_PointA06_0007_ChannelDAPI,WF_GFP,TRITC,WF_Cy5,DIA_Seq0052.h5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">second_pass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plateK10rep1_20200429_122048_065_WellG06_PointG06_0005_ChannelDAPI,WF_GFP,TRITC,WF_Cy5,DIA_Seq0662.h5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plateK10rep1_20200429_122048_065_WellH02_PointH02_0003_ChannelDAPI,WF_GFP,TRITC,WF_Cy5,DIA_Seq0813.h5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plateK11rep1_20200429_140316_208_WellD05_PointD05_0007_ChannelDAPI,WF_GFP,TRITC,WF_Cy5,DIA_Seq0394.h5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plateK11rep1_20200429_140316_208_WellE05_PointE05_0004_ChannelDAPI,WF_GFP,TRITC,WF_Cy5,DIA_Seq0454.h5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plateK11rep1_20200429_140316_208_WellH06_PointH06_0006_ChannelDAPI,WF_GFP,TRITC,WF_Cy5,DIA_Seq0780.h5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plateK12rep1_20200430_155932_313_WellC08_PointC08_0000_ChannelDAPI,WF_GFP,TRITC,WF_Cy5,DIA_Seq0279.h5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plateK12rep1_20200430_155932_313_WellD09_PointD09_0003_ChannelDAPI,WF_GFP,TRITC,WF_Cy5,DIA_Seq0354.h5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plateK12rep1_20200430_155932_313_WellF04_PointF04_0002_ChannelDAPI,WF_GFP,TRITC,WF_Cy5,DIA_Seq0614.h5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plateK13rep1_20200430_175056_461_WellA10_PointA10_0007_ChannelDAPI,WF_GFP,TRITC,WF_Cy5,DIA_Seq0088.h5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plateK13rep1_20200430_175056_461_WellE04_PointE04_0000_ChannelDAPI,WF_GFP,TRITC,WF_Cy5,DIA_Seq0108.h5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plateK13rep1_20200430_175056_461_WellF02_PointF02_0008_ChannelDAPI,WF_GFP,TRITC,WF_Cy5,DIA_Seq0161.h5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plateK13rep1_20200430_175056_461_WellF08_PointF08_0008_ChannelDAPI,WF_GFP,TRITC,WF_Cy5,DIA_Seq0215.h5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plateK14rep1_20200430_194338_941_WellE09_PointE09_0002_ChannelDAPI,WF_GFP,TRITC,WF_Cy5,DIA_Seq0506.h5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plateK14rep1_20200430_194338_941_WellF02_PointF02_0003_ChannelDAPI,WF_GFP,TRITC,WF_Cy5,DIA_Seq0633.h5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plateK14rep1_20200430_194338_941_WellG04_PointG04_0008_ChannelDAPI,WF_GFP,TRITC,WF_Cy5,DIA_Seq0683.h5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">titration_plate_20200403_154849_WellD01_PointD01_0004_ChannelDAPI,WF_GFP,TRITC,WF_Cy5_Seq0427.h5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">titration_plate_20200403_154849_WellD10_PointD10_0006_ChannelDAPI,WF_GFP,TRITC,WF_Cy5_Seq0348.h5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">titration_plate_20200403_154849_WellH08_PointH08_0008_ChannelDAPI,WF_GFP,TRITC,WF_Cy5_Seq0800.h5</t>
   </si>
 </sst>
 </file>
@@ -201,10 +261,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B53" activeCellId="0" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -485,6 +545,158 @@
         <v>5</v>
       </c>
     </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Add functionality for more systematic proof-reading
</commit_message>
<xml_diff>
--- a/annotation_status.xlsx
+++ b/annotation_status.xlsx
@@ -106,19 +106,19 @@
     <t xml:space="preserve">plateK10rep1_20200429_122048_065_WellA06_PointA06_0007_ChannelDAPI,WF_GFP,TRITC,WF_Cy5,DIA_Seq0052.h5</t>
   </si>
   <si>
+    <t xml:space="preserve">plateK10rep1_20200429_122048_065_WellG06_PointG06_0005_ChannelDAPI,WF_GFP,TRITC,WF_Cy5,DIA_Seq0662.h5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plateK10rep1_20200429_122048_065_WellH02_PointH02_0003_ChannelDAPI,WF_GFP,TRITC,WF_Cy5,DIA_Seq0813.h5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plateK11rep1_20200429_140316_208_WellD05_PointD05_0007_ChannelDAPI,WF_GFP,TRITC,WF_Cy5,DIA_Seq0394.h5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plateK11rep1_20200429_140316_208_WellE05_PointE05_0004_ChannelDAPI,WF_GFP,TRITC,WF_Cy5,DIA_Seq0454.h5</t>
+  </si>
+  <si>
     <t xml:space="preserve">second_pass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plateK10rep1_20200429_122048_065_WellG06_PointG06_0005_ChannelDAPI,WF_GFP,TRITC,WF_Cy5,DIA_Seq0662.h5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plateK10rep1_20200429_122048_065_WellH02_PointH02_0003_ChannelDAPI,WF_GFP,TRITC,WF_Cy5,DIA_Seq0813.h5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plateK11rep1_20200429_140316_208_WellD05_PointD05_0007_ChannelDAPI,WF_GFP,TRITC,WF_Cy5,DIA_Seq0394.h5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plateK11rep1_20200429_140316_208_WellE05_PointE05_0004_ChannelDAPI,WF_GFP,TRITC,WF_Cy5,DIA_Seq0454.h5</t>
   </si>
   <si>
     <t xml:space="preserve">plateK11rep1_20200429_140316_208_WellH06_PointH06_0006_ChannelDAPI,WF_GFP,TRITC,WF_Cy5,DIA_Seq0780.h5</t>
@@ -263,8 +263,8 @@
   </sheetPr>
   <dimension ref="A1:B53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B53" activeCellId="0" sqref="B53"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B38" activeCellId="0" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -550,20 +550,20 @@
         <v>27</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B37" s="0" t="s">
         <v>5</v>
@@ -571,18 +571,18 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -590,7 +590,7 @@
         <v>33</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -598,7 +598,7 @@
         <v>34</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -606,7 +606,7 @@
         <v>35</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -614,7 +614,7 @@
         <v>36</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -622,7 +622,7 @@
         <v>37</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -638,7 +638,7 @@
         <v>39</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -646,7 +646,7 @@
         <v>40</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -654,7 +654,7 @@
         <v>41</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -662,7 +662,7 @@
         <v>42</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -670,7 +670,7 @@
         <v>43</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -678,7 +678,7 @@
         <v>44</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -686,7 +686,7 @@
         <v>45</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -694,7 +694,7 @@
         <v>46</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>